<commit_message>
removed customers xcel file and copied over to vendors
</commit_message>
<xml_diff>
--- a/Vendors p0.xlsx
+++ b/Vendors p0.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\p0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C8FE7AA-30DC-409A-9857-A55DEB2F042D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88FDEA4D-C696-4315-88CD-0ACD83A89059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EEEA010D-CE0C-4C9D-8732-434099618153}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EEEA010D-CE0C-4C9D-8732-434099618153}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -83,6 +84,15 @@
   </si>
   <si>
     <t>Laptop</t>
+  </si>
+  <si>
+    <t>Shopping List</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Bob</t>
   </si>
 </sst>
 </file>
@@ -436,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9C8054-4E5F-46C8-B771-8A0684CC76AD}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,4 +717,48 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5910A2-DFB3-4F54-9AD2-B905534401B8}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added new variables and worked towards deducting stock and totaling expense for each customer item
</commit_message>
<xml_diff>
--- a/Vendors p0.xlsx
+++ b/Vendors p0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\p0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5470BAA-881E-4AB6-BE92-AE32AECA80E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F5A9E3-572D-4608-ABE8-17A6E8869027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EEEA010D-CE0C-4C9D-8732-434099618153}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
   <si>
     <t>Socks</t>
   </si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Discount</t>
   </si>
 </sst>
 </file>
@@ -457,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9C8054-4E5F-46C8-B771-8A0684CC76AD}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,26 +474,29 @@
     <col min="7" max="7" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B2" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -501,13 +504,16 @@
       <c r="D2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>1.25</v>
@@ -515,13 +521,16 @@
       <c r="D3">
         <v>99</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <v>4.5</v>
@@ -529,13 +538,16 @@
       <c r="D4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>1.5</v>
@@ -543,13 +555,16 @@
       <c r="D5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -557,13 +572,16 @@
       <c r="D6">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -571,13 +589,16 @@
       <c r="D7">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>500</v>
@@ -585,13 +606,16 @@
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -599,33 +623,42 @@
       <c r="D9">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10">
         <v>200</v>
       </c>
       <c r="D10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <v>800</v>
       </c>
       <c r="D11">
         <v>1</v>
+      </c>
+      <c r="E11">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -649,21 +682,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -671,10 +704,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -682,10 +715,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -693,10 +726,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -704,10 +737,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -715,10 +748,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -726,10 +759,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>20</v>
@@ -737,10 +770,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9">
         <v>20</v>
@@ -748,10 +781,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>20</v>
@@ -779,10 +812,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
save expense of items in hashtable clientExpenses and deduct stock in intentory datatable
</commit_message>
<xml_diff>
--- a/Vendors p0.xlsx
+++ b/Vendors p0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\p0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F5A9E3-572D-4608-ABE8-17A6E8869027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8A5209-ABA6-4AD8-8E89-A8966C81038E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EEEA010D-CE0C-4C9D-8732-434099618153}"/>
   </bookViews>
@@ -460,7 +460,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,10 +536,10 @@
         <v>4.5</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -553,10 +553,10 @@
         <v>1.5</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E5">
-        <v>7.5</v>
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -570,10 +570,10 @@
         <v>6</v>
       </c>
       <c r="D6">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="E6">
-        <v>20</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -590,7 +590,7 @@
         <v>100</v>
       </c>
       <c r="E7">
-        <v>35</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -604,7 +604,7 @@
         <v>500</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -621,10 +621,10 @@
         <v>5</v>
       </c>
       <c r="D9">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -658,7 +658,7 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>15</v>
+        <v>0.15</v>
       </c>
     </row>
   </sheetData>
@@ -671,7 +671,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
successfully writes expense sheet and updates stock
</commit_message>
<xml_diff>
--- a/Vendors p0.xlsx
+++ b/Vendors p0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\p0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8A5209-ABA6-4AD8-8E89-A8966C81038E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0169EE24-7AA3-45B6-8EA0-C7DF59DDDB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EEEA010D-CE0C-4C9D-8732-434099618153}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
   <si>
     <t>Socks</t>
   </si>
@@ -72,6 +72,30 @@
     <t>Item</t>
   </si>
   <si>
+    <t>Walmart</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Webb</t>
+  </si>
+  <si>
+    <t>Joe</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
     <t>Vendor</t>
   </si>
   <si>
@@ -79,30 +103,6 @@
   </si>
   <si>
     <t>Stock</t>
-  </si>
-  <si>
-    <t>Walmart</t>
-  </si>
-  <si>
-    <t>Amazon</t>
-  </si>
-  <si>
-    <t>Target</t>
-  </si>
-  <si>
-    <t>Client</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Webb</t>
-  </si>
-  <si>
-    <t>Joe</t>
-  </si>
-  <si>
-    <t>Total</t>
   </si>
   <si>
     <t>Discount</t>
@@ -460,7 +460,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,13 +479,13 @@
         <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
         <v>23</v>
@@ -496,13 +496,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>10</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -513,13 +513,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>1.25</v>
       </c>
       <c r="D3">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -530,7 +530,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>4.5</v>
@@ -547,13 +547,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>1.5</v>
       </c>
       <c r="D5">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E5">
         <v>7.4999999999999997E-2</v>
@@ -564,13 +564,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>6</v>
       </c>
       <c r="D6">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="E6">
         <v>0.2</v>
@@ -581,13 +581,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E7">
         <v>0.35</v>
@@ -598,13 +598,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>500</v>
       </c>
       <c r="D8">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -615,7 +615,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -632,13 +632,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>200</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -649,7 +649,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>800</v>
@@ -682,13 +682,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -726,7 +726,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -737,7 +737,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -748,7 +748,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -759,7 +759,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -770,7 +770,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -781,7 +781,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -797,7 +797,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1BA319-E0B0-4FA0-ADC0-95BEB828573A}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -812,10 +812,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>211.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
-        <v>22</v>
+      <c r="B4">
+        <v>78.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
seperated shopping sequence from main
</commit_message>
<xml_diff>
--- a/Vendors p0.xlsx
+++ b/Vendors p0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\p0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0169EE24-7AA3-45B6-8EA0-C7DF59DDDB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FECFA4-D447-49E7-9776-9709886AA296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EEEA010D-CE0C-4C9D-8732-434099618153}"/>
   </bookViews>
@@ -460,7 +460,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +502,7 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -519,7 +519,7 @@
         <v>1.25</v>
       </c>
       <c r="D3">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -553,7 +553,7 @@
         <v>1.5</v>
       </c>
       <c r="D5">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <v>7.4999999999999997E-2</v>
@@ -570,7 +570,7 @@
         <v>6</v>
       </c>
       <c r="D6">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E6">
         <v>0.2</v>
@@ -587,7 +587,7 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="E7">
         <v>0.35</v>
@@ -638,7 +638,7 @@
         <v>200</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>0</v>

</xml_diff>

<commit_message>
added items not found sheet and writes to it when no stock or item not found in datatable
</commit_message>
<xml_diff>
--- a/Vendors p0.xlsx
+++ b/Vendors p0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\p0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FECFA4-D447-49E7-9776-9709886AA296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8191023E-94DC-4FAE-B8B4-B63BF5272A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EEEA010D-CE0C-4C9D-8732-434099618153}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
     <sheet name="Shopping List" sheetId="2" r:id="rId2"/>
     <sheet name="Expenses" sheetId="3" r:id="rId3"/>
+    <sheet name="Items Not Found" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="28">
   <si>
     <t>Socks</t>
   </si>
@@ -106,6 +107,18 @@
   </si>
   <si>
     <t>Discount</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>sdfsdfsdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unaccounted Quantity </t>
   </si>
 </sst>
 </file>
@@ -460,7 +473,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +515,7 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>999</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -519,7 +532,7 @@
         <v>1.25</v>
       </c>
       <c r="D3">
-        <v>53</v>
+        <v>977</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -536,7 +549,7 @@
         <v>4.5</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="E4">
         <v>0.05</v>
@@ -553,7 +566,7 @@
         <v>1.5</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>980</v>
       </c>
       <c r="E5">
         <v>7.4999999999999997E-2</v>
@@ -570,7 +583,7 @@
         <v>6</v>
       </c>
       <c r="D6">
-        <v>64</v>
+        <v>9998</v>
       </c>
       <c r="E6">
         <v>0.2</v>
@@ -587,7 +600,7 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>60</v>
+        <v>9980</v>
       </c>
       <c r="E7">
         <v>0.35</v>
@@ -604,7 +617,7 @@
         <v>500</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -621,7 +634,7 @@
         <v>5</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="E9">
         <v>0.02</v>
@@ -638,7 +651,7 @@
         <v>200</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -668,10 +681,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5910A2-DFB3-4F54-9AD2-B905534401B8}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,13 +706,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -707,7 +720,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -718,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -726,13 +739,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
         <v>1</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -740,10 +753,10 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -751,21 +764,21 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -773,7 +786,7 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>20</v>
@@ -784,9 +797,20 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>20</v>
       </c>
     </row>
@@ -831,7 +855,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>12.1</v>
+        <v>36.6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -840,6 +864,48 @@
       </c>
       <c r="B4">
         <v>78.75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA6B651-4C05-4A26-8D8F-203B9D316C7A}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed break into continue
</commit_message>
<xml_diff>
--- a/Vendors p0.xlsx
+++ b/Vendors p0.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\p0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8191023E-94DC-4FAE-B8B4-B63BF5272A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B83AFB-6966-4620-9E79-2ACD5007DFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EEEA010D-CE0C-4C9D-8732-434099618153}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{EEEA010D-CE0C-4C9D-8732-434099618153}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
     <sheet name="Shopping List" sheetId="2" r:id="rId2"/>
-    <sheet name="Expenses" sheetId="3" r:id="rId3"/>
-    <sheet name="Items Not Found" sheetId="4" r:id="rId4"/>
+    <sheet name="Expenses" sheetId="6" r:id="rId3"/>
+    <sheet name="Items Not Found" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="27">
   <si>
     <t>Socks</t>
   </si>
@@ -94,31 +94,28 @@
     <t>Joe</t>
   </si>
   <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>Unaccounted Quantity</t>
+  </si>
+  <si>
     <t>Total</t>
   </si>
   <si>
-    <t>Vendor</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Stock</t>
-  </si>
-  <si>
-    <t>Discount</t>
-  </si>
-  <si>
     <t>Jane</t>
   </si>
   <si>
     <t>sdfsdfsdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Item </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unaccounted Quantity </t>
   </si>
 </sst>
 </file>
@@ -472,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9C8054-4E5F-46C8-B771-8A0684CC76AD}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,16 +489,16 @@
         <v>11</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>22</v>
-      </c>
-      <c r="E1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -515,7 +512,7 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -532,7 +529,7 @@
         <v>1.25</v>
       </c>
       <c r="D3">
-        <v>977</v>
+        <v>908</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -566,7 +563,7 @@
         <v>1.5</v>
       </c>
       <c r="D5">
-        <v>980</v>
+        <v>920</v>
       </c>
       <c r="E5">
         <v>7.4999999999999997E-2</v>
@@ -583,7 +580,7 @@
         <v>6</v>
       </c>
       <c r="D6">
-        <v>9998</v>
+        <v>9992</v>
       </c>
       <c r="E6">
         <v>0.2</v>
@@ -600,7 +597,7 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>9980</v>
+        <v>9920</v>
       </c>
       <c r="E7">
         <v>0.35</v>
@@ -634,7 +631,7 @@
         <v>5</v>
       </c>
       <c r="D9">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="E9">
         <v>0.02</v>
@@ -651,7 +648,7 @@
         <v>200</v>
       </c>
       <c r="D10">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -684,7 +681,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,13 +703,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -720,7 +717,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -731,7 +728,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -739,13 +736,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -753,21 +750,21 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -820,18 +817,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1BA319-E0B0-4FA0-ADC0-95BEB828573A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C3FB73A-AED5-4476-B778-BB75CA353500}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -839,7 +835,7 @@
         <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -872,7 +868,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA6B651-4C05-4A26-8D8F-203B9D316C7A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7819EE-1D2B-4DD4-B7CC-C2F33679973C}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -881,9 +877,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -891,21 +887,21 @@
         <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug with counting negative stock
</commit_message>
<xml_diff>
--- a/Vendors p0.xlsx
+++ b/Vendors p0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\p0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B83AFB-6966-4620-9E79-2ACD5007DFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2456225-320A-4AF0-903D-AF848C4B58A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{EEEA010D-CE0C-4C9D-8732-434099618153}"/>
+    <workbookView xWindow="1515" yWindow="1485" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{EEEA010D-CE0C-4C9D-8732-434099618153}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="27">
   <si>
     <t>Socks</t>
   </si>
@@ -470,7 +470,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,7 +512,7 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>996</v>
+        <v>991</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -529,7 +529,7 @@
         <v>1.25</v>
       </c>
       <c r="D3">
-        <v>908</v>
+        <v>793</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -563,7 +563,7 @@
         <v>1.5</v>
       </c>
       <c r="D5">
-        <v>920</v>
+        <v>820</v>
       </c>
       <c r="E5">
         <v>7.4999999999999997E-2</v>
@@ -580,7 +580,7 @@
         <v>6</v>
       </c>
       <c r="D6">
-        <v>9992</v>
+        <v>9982</v>
       </c>
       <c r="E6">
         <v>0.2</v>
@@ -597,7 +597,7 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>9920</v>
+        <v>9820</v>
       </c>
       <c r="E7">
         <v>0.35</v>
@@ -631,7 +631,7 @@
         <v>5</v>
       </c>
       <c r="D9">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="E9">
         <v>0.02</v>
@@ -648,7 +648,7 @@
         <v>200</v>
       </c>
       <c r="D10">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -665,7 +665,7 @@
         <v>800</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>0.15</v>
@@ -678,10 +678,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5910A2-DFB3-4F54-9AD2-B905534401B8}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,6 +811,17 @@
         <v>20</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -821,7 +832,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B4" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,7 +870,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>78.75</v>
+        <v>758.75</v>
       </c>
     </row>
   </sheetData>
@@ -869,10 +880,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7819EE-1D2B-4DD4-B7CC-C2F33679973C}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,6 +915,17 @@
         <v>51</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
delete all cells in expenses and items not found sheets before writing to it in shop.xaml
</commit_message>
<xml_diff>
--- a/Vendors p0.xlsx
+++ b/Vendors p0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\p0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2456225-320A-4AF0-903D-AF848C4B58A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC0D81A-208A-4105-89E7-5215DA8F5A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1485" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{EEEA010D-CE0C-4C9D-8732-434099618153}"/>
+    <workbookView xWindow="1515" yWindow="1485" windowWidth="21600" windowHeight="11385" xr2:uid="{EEEA010D-CE0C-4C9D-8732-434099618153}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -469,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9C8054-4E5F-46C8-B771-8A0684CC76AD}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,7 +512,7 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>991</v>
+        <v>983</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -529,7 +529,7 @@
         <v>1.25</v>
       </c>
       <c r="D3">
-        <v>793</v>
+        <v>609</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -563,7 +563,7 @@
         <v>1.5</v>
       </c>
       <c r="D5">
-        <v>820</v>
+        <v>660</v>
       </c>
       <c r="E5">
         <v>7.4999999999999997E-2</v>
@@ -580,7 +580,7 @@
         <v>6</v>
       </c>
       <c r="D6">
-        <v>9982</v>
+        <v>9966</v>
       </c>
       <c r="E6">
         <v>0.2</v>
@@ -597,7 +597,7 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>9820</v>
+        <v>9660</v>
       </c>
       <c r="E7">
         <v>0.35</v>
@@ -631,7 +631,7 @@
         <v>5</v>
       </c>
       <c r="D9">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="E9">
         <v>0.02</v>
@@ -648,7 +648,7 @@
         <v>200</v>
       </c>
       <c r="D10">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -831,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C3FB73A-AED5-4476-B778-BB75CA353500}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="A2:B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="A2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,7 +883,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D4" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
worked on adding stock to vendors
</commit_message>
<xml_diff>
--- a/Vendors p0.xlsx
+++ b/Vendors p0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revature\p0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Rymarz_N-Wilson_D-p0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFAFEA1-EF1D-459B-BBCE-DD610A17C42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A613FC-DA94-4743-96F9-0F9078E77242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{EEEA010D-CE0C-4C9D-8732-434099618153}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{EEEA010D-CE0C-4C9D-8732-434099618153}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>T.V</t>
   </si>
   <si>
-    <t>Laptop</t>
-  </si>
-  <si>
     <t>Bob</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>sdfsdfsdf</t>
+  </si>
+  <si>
+    <t>Laptops</t>
   </si>
 </sst>
 </file>
@@ -462,44 +462,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9C8054-4E5F-46C8-B771-8A0684CC76AD}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" customWidth="1"/>
-    <col min="6" max="6" width="21.5546875" customWidth="1"/>
-    <col min="7" max="7" width="23.5546875" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -511,12 +511,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>1.25</v>
@@ -528,12 +528,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>4.5</v>
@@ -545,12 +545,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>1.5</v>
@@ -562,12 +562,12 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -579,12 +579,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -596,12 +596,12 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>500</v>
@@ -613,12 +613,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -630,12 +630,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>200</v>
@@ -647,12 +647,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>800</v>
@@ -677,26 +677,26 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -705,9 +705,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -716,9 +716,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -727,9 +727,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -738,9 +738,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -749,20 +749,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
         <v>25</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
       </c>
       <c r="C7">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -771,9 +771,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -782,9 +782,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
@@ -793,9 +793,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -813,43 +813,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C3FB73A-AED5-4476-B778-BB75CA353500}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>211.25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>36.6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>78.75</v>
@@ -868,30 +868,30 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
         <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
       </c>
       <c r="C2">
         <v>51</v>

</xml_diff>

<commit_message>
adding stock to vendors works
</commit_message>
<xml_diff>
--- a/Vendors p0.xlsx
+++ b/Vendors p0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Rymarz_N-Wilson_D-p0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A613FC-DA94-4743-96F9-0F9078E77242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE20C0D-205E-4F15-835F-FE8C6A76FB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{EEEA010D-CE0C-4C9D-8732-434099618153}"/>
+    <workbookView xWindow="-21510" yWindow="2565" windowWidth="21600" windowHeight="11385" xr2:uid="{EEEA010D-CE0C-4C9D-8732-434099618153}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -463,7 +463,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +590,7 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>9800</v>
+        <v>9850</v>
       </c>
       <c r="E7">
         <v>0.35</v>
@@ -624,7 +624,7 @@
         <v>5</v>
       </c>
       <c r="D9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E9">
         <v>0.02</v>
@@ -658,7 +658,7 @@
         <v>800</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E11">
         <v>0.15</v>

</xml_diff>

<commit_message>
fixed bug with shop not correclty counting unaccounted for stock and renamed cases for starting input dialog switch flow. added the add stock pprompt to its own xaml
</commit_message>
<xml_diff>
--- a/Vendors p0.xlsx
+++ b/Vendors p0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Rymarz_N-Wilson_D-p0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE20C0D-205E-4F15-835F-FE8C6A76FB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2C03C2-A0FA-4E11-A522-6C85A09B9010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21510" yWindow="2565" windowWidth="21600" windowHeight="11385" xr2:uid="{EEEA010D-CE0C-4C9D-8732-434099618153}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{EEEA010D-CE0C-4C9D-8732-434099618153}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="28">
   <si>
     <t>Socks</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Laptops</t>
+  </si>
+  <si>
+    <t>Bill</t>
   </si>
 </sst>
 </file>
@@ -463,7 +466,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,7 +508,7 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -522,7 +525,7 @@
         <v>1.25</v>
       </c>
       <c r="D3">
-        <v>770</v>
+        <v>701</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -556,7 +559,7 @@
         <v>1.5</v>
       </c>
       <c r="D5">
-        <v>800</v>
+        <v>740</v>
       </c>
       <c r="E5">
         <v>7.4999999999999997E-2</v>
@@ -573,7 +576,7 @@
         <v>6</v>
       </c>
       <c r="D6">
-        <v>9980</v>
+        <v>9974</v>
       </c>
       <c r="E6">
         <v>0.2</v>
@@ -590,7 +593,7 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>9850</v>
+        <v>9790</v>
       </c>
       <c r="E7">
         <v>0.35</v>
@@ -624,7 +627,7 @@
         <v>5</v>
       </c>
       <c r="D9">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="E9">
         <v>0.02</v>
@@ -641,7 +644,7 @@
         <v>200</v>
       </c>
       <c r="D10">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -658,7 +661,7 @@
         <v>800</v>
       </c>
       <c r="D11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11">
         <v>0.15</v>
@@ -671,10 +674,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5910A2-DFB3-4F54-9AD2-B905534401B8}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,6 +807,17 @@
         <v>20</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -811,10 +825,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C3FB73A-AED5-4476-B778-BB75CA353500}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,6 +869,14 @@
         <v>78.75</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>3400</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -862,7 +884,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7819EE-1D2B-4DD4-B7CC-C2F33679973C}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -897,6 +919,17 @@
         <v>51</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>